<commit_message>
documentation (image, rename etc)
</commit_message>
<xml_diff>
--- a/Documentation/Test.xlsx
+++ b/Documentation/Test.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sven.VOLERY\Documents\GitHub\PROJ-Annonces\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yann7\Documents\GitHub\PROJ-Annonces\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0126B800-0813-41BD-BFF4-7634CF5F8C96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView minimized="1" xWindow="1188" yWindow="1188" windowWidth="17280" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="22">
   <si>
     <t>Scénario</t>
   </si>
@@ -41,40 +42,61 @@
     <t>OK</t>
   </si>
   <si>
-    <t>Rentrer les champs (users, Email, Password)</t>
-  </si>
-  <si>
-    <t>Bouton "Inscrivez-vous" pour inscrire le compte</t>
-  </si>
-  <si>
-    <t>Afficher la page "Login"</t>
-  </si>
-  <si>
-    <t>Rentrer les champs d'un compte créé auparavant</t>
-  </si>
-  <si>
-    <t>Bouton "Connexion" pour se connecter au compte</t>
-  </si>
-  <si>
-    <t>Afficher la page "+" en étant connecter à un compte</t>
-  </si>
-  <si>
-    <t>Rentrer les champs pour créer une annonces</t>
-  </si>
-  <si>
-    <t>Bouton "valider" pour poster l'annonce</t>
-  </si>
-  <si>
-    <t>Bouton "modifier" affiche le formulaire de l'annonce</t>
-  </si>
-  <si>
-    <t>Bouton "supprimer" pour supprimer l'annonce</t>
+    <t>S'inscrire</t>
+  </si>
+  <si>
+    <t>Redirection vers l'acceuil</t>
+  </si>
+  <si>
+    <t>Se déconnecter</t>
+  </si>
+  <si>
+    <t>Se connecter</t>
+  </si>
+  <si>
+    <t>Voir les annonces après connexion</t>
+  </si>
+  <si>
+    <t>Ajouter une annonce</t>
+  </si>
+  <si>
+    <t>Accèder au formulaire d'ajout d'annonce</t>
+  </si>
+  <si>
+    <t>Voir l'annonce postée</t>
+  </si>
+  <si>
+    <t>Accèder aux détails de l'annonce</t>
+  </si>
+  <si>
+    <t>Accèder à la modification de l'annonce</t>
+  </si>
+  <si>
+    <t>Modifier l'annoncer (et vérifier qu'elle a bien été modifiée)</t>
+  </si>
+  <si>
+    <t>Voir les autres annonces et contacter le posteurs d'une autre annonce</t>
+  </si>
+  <si>
+    <t>Accèder à l'acceuil</t>
+  </si>
+  <si>
+    <t>Fanha Yann</t>
+  </si>
+  <si>
+    <t>Navigateurs</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>Firefox</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -100,7 +122,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,8 +159,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -177,11 +205,75 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -189,41 +281,77 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -504,256 +632,370 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="54.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="7" t="s">
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="11" t="s">
+      <c r="D4" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="5">
-        <v>44284</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="10">
+        <v>44284</v>
+      </c>
+      <c r="D6" s="16">
+        <v>44286</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="5">
-        <v>44284</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="4"/>
-      <c r="C7" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+      <c r="C8" s="10">
+        <v>44284</v>
+      </c>
+      <c r="D8" s="16">
+        <v>44286</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="8"/>
+      <c r="C9" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="5">
-        <v>44284</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="11"/>
-      <c r="C9" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="10">
+        <v>44284</v>
+      </c>
+      <c r="D10" s="16">
+        <v>44286</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="7"/>
+      <c r="C11" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="5">
-        <v>44284</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="4"/>
-      <c r="C11" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
+      <c r="C12" s="10">
+        <v>44284</v>
+      </c>
+      <c r="D12" s="16">
+        <v>44286</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="8"/>
+      <c r="C13" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="5">
-        <v>44284</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="11"/>
-      <c r="C13" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="8" t="s">
+      <c r="C14" s="10">
+        <v>44284</v>
+      </c>
+      <c r="D14" s="16">
+        <v>44286</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="7"/>
+      <c r="C15" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="9">
-        <v>44284</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="8"/>
-      <c r="C15" s="10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="12" t="s">
+      <c r="C16" s="12">
+        <v>44284</v>
+      </c>
+      <c r="D16" s="16">
+        <v>44286</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="6"/>
+      <c r="C17" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="9">
-        <v>44284</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="12"/>
-      <c r="C17" s="10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="8" t="s">
+      <c r="C18" s="12">
+        <v>44284</v>
+      </c>
+      <c r="D18" s="16">
+        <v>44286</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="5"/>
+      <c r="C19" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="14">
+        <v>44284</v>
+      </c>
+      <c r="D20" s="16">
+        <v>44286</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="6"/>
+      <c r="C21" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="14">
-        <v>44284</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="8"/>
-      <c r="C19" s="10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="14">
-        <v>44284</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="12"/>
-      <c r="C21" s="10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="8" t="s">
+      <c r="C22" s="14">
+        <v>44284</v>
+      </c>
+      <c r="D22" s="16">
+        <v>44286</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="5"/>
+      <c r="C23" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="14">
-        <v>44284</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="8"/>
-      <c r="C23" s="10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="12" t="s">
+      <c r="C24" s="14">
+        <v>44284</v>
+      </c>
+      <c r="D24" s="16">
+        <v>44286</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25" s="6"/>
+      <c r="C25" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B26" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="14">
-        <v>44284</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="12"/>
-      <c r="C25" s="10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="8" t="s">
+      <c r="C26" s="14">
+        <v>44284</v>
+      </c>
+      <c r="D26" s="16">
+        <v>44286</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B27" s="5"/>
+      <c r="C27" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B28" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="14">
-        <v>44284</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="8"/>
-      <c r="C27" s="10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
+      <c r="C28" s="14">
+        <v>44284</v>
+      </c>
+      <c r="D28" s="16">
+        <v>44286</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B29" s="21"/>
+      <c r="C29" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B30" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="14">
+        <v>44284</v>
+      </c>
+      <c r="D30" s="16">
+        <v>44286</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B31" s="5"/>
+      <c r="C31" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B32" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="14">
+        <v>44284</v>
+      </c>
+      <c r="D32" s="16">
+        <v>44286</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B33" s="22"/>
+      <c r="C33" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B34" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="14">
+        <v>44284</v>
+      </c>
+      <c r="D34" s="16">
+        <v>44286</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="23"/>
+      <c r="C35" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="15">
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
     <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B34:B35"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>